<commit_message>
Homelessness widgets and uploader.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_rentalstress_uploader/housing_rentalstress.xlsx
+++ b/dashboard_loader/housing_rentalstress_uploader/housing_rentalstress.xlsx
@@ -730,7 +730,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -764,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>21</v>
       </c>
@@ -772,7 +772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>23</v>
       </c>
@@ -780,7 +780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="9" t="s">
         <v>25</v>
       </c>
@@ -795,7 +795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="9" t="s">
         <v>28</v>
       </c>

</xml_diff>